<commit_message>
Added forecast analysis methods Brown Holt
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/test.xlsx
+++ b/spec/fixtures/files/test.xlsx
@@ -41,6 +41,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,13 +101,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -126,16 +131,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -149,264 +151,160 @@
       <c r="A2" s="1" t="n">
         <v>42566</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>106.85</v>
+      <c r="B2" s="2" t="n">
+        <v>106.94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>42569</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>108.55</v>
+      <c r="B3" s="2" t="n">
+        <v>106.82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>42570</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>107.56</v>
+      <c r="B4" s="2" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>42571</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>108.1</v>
+      <c r="B5" s="2" t="n">
+        <v>106.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>42572</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>108.93</v>
+      <c r="B6" s="2" t="n">
+        <v>106.73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>42573</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>111.71</v>
+      <c r="B7" s="2" t="n">
+        <v>107.73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>42576</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>108.18</v>
+      <c r="B8" s="2" t="n">
+        <v>107.7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>42577</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>103.69</v>
+      <c r="B9" s="2" t="n">
+        <v>108.36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>42578</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>98.89</v>
+      <c r="B10" s="2" t="n">
+        <v>105.52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>42579</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>88.34</v>
+      <c r="B11" s="2" t="n">
+        <v>103.13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>42580</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>80.21</v>
+      <c r="B12" s="2" t="n">
+        <v>105.44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>42583</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>63.43</v>
+      <c r="B13" s="2" t="n">
+        <v>107.95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>42584</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>50.04</v>
+      <c r="B14" s="2" t="n">
+        <v>111.77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>42585</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>59.56</v>
+      <c r="B15" s="2" t="n">
+        <v>115.57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>42586</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>57.11</v>
+      <c r="B16" s="2" t="n">
+        <v>114.92</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>42587</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>61.58</v>
+      <c r="B17" s="2" t="n">
+        <v>113.58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>42590</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <v>65.91</v>
+      <c r="B18" s="2" t="n">
+        <v>113.57</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>42591</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>63.97</v>
+      <c r="B19" s="2" t="n">
+        <v>113.55</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>42592</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>56.89</v>
+      <c r="B20" s="2" t="n">
+        <v>114.62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>42593</v>
       </c>
-      <c r="B21" s="0" t="n">
-        <v>48.32</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>42594</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>48.66</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>42597</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>49.54</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>42598</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>46.02</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>42599</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>39.02</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
-        <v>42600</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>32.13</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>42601</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>33.66</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>42604</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>42605</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>43.28</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>42607</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>47.78</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>42608</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>49.87</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>42611</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>46.69</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>42612</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>47.28</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>42613</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>47.47</v>
+      <c r="B21" s="2" t="n">
+        <v>112.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>